<commit_message>
Update the attendance function
</commit_message>
<xml_diff>
--- a/2023_11.xlsx
+++ b/2023_11.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Month</t>
   </si>
@@ -31,16 +31,22 @@
     <t>Check In Status</t>
   </si>
   <si>
+    <t>Check In Time</t>
+  </si>
+  <si>
     <t>Check Out</t>
   </si>
   <si>
     <t>Check Out Status</t>
   </si>
   <si>
+    <t>Check Out Time</t>
+  </si>
+  <si>
     <t>Total Salary</t>
   </si>
   <si>
-    <t>2023-11-06</t>
+    <t>11/7/2023</t>
   </si>
   <si>
     <t>ThaiNX</t>
@@ -52,13 +58,28 @@
     <t>on time</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>8:54</t>
+  </si>
+  <si>
+    <t>19:55</t>
   </si>
   <si>
     <t>Thanh Ha</t>
   </si>
   <si>
-    <t>Duy Long</t>
+    <t>late</t>
+  </si>
+  <si>
+    <t>10:55</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>21:56</t>
   </si>
 </sst>
 </file>
@@ -435,15 +456,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="9" width="15" customWidth="1"/>
+    <col min="5" max="11" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,79 +492,74 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2">
-        <v>500000</v>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3">
         <v>500000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update auto check attendance
</commit_message>
<xml_diff>
--- a/2023_11.xlsx
+++ b/2023_11.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
   <si>
     <t>Month</t>
   </si>
@@ -46,7 +46,7 @@
     <t>Total Salary</t>
   </si>
   <si>
-    <t>11/7/2023</t>
+    <t>11/9/2023</t>
   </si>
   <si>
     <t>ThaiNX</t>
@@ -58,28 +58,52 @@
     <t>on time</t>
   </si>
   <si>
-    <t>8:54</t>
-  </si>
-  <si>
-    <t>19:55</t>
+    <t>8:48</t>
+  </si>
+  <si>
+    <t>20:49</t>
+  </si>
+  <si>
+    <t>11/10/2023</t>
+  </si>
+  <si>
+    <t>8:53</t>
+  </si>
+  <si>
+    <t>19:24</t>
+  </si>
+  <si>
+    <t>11/11/2023</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>12:02</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>Thanh Ha</t>
   </si>
   <si>
+    <t>Duy Long</t>
+  </si>
+  <si>
+    <t>11/12/2023</t>
+  </si>
+  <si>
     <t>late</t>
   </si>
   <si>
-    <t>10:55</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>missing</t>
-  </si>
-  <si>
-    <t>21:56</t>
+    <t>10:42</t>
+  </si>
+  <si>
+    <t>20:43</t>
   </si>
 </sst>
 </file>
@@ -456,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="3" width="15" customWidth="1"/>
@@ -535,32 +559,221 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3">
-        <v>500000</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9">
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>